<commit_message>
Prepare 4 additional test cases for Bofidi
</commit_message>
<xml_diff>
--- a/excel_tax_calculation/input_output/input_output_overview.xlsx
+++ b/excel_tax_calculation/input_output/input_output_overview.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benjamin.van.dam/Documents/codebases/be_market/excel_tax_calculation/input_output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FD73F04-4118-2A46-8EA3-C811085A3D22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{806E30C0-E8B6-A147-B2E3-D77ED876C224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="16280" xr2:uid="{B5C74626-8E96-454A-A0EA-D4ED5FC94566}"/>
   </bookViews>
@@ -63,7 +63,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -83,6 +86,13 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -101,23 +111,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -450,17 +462,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D0DD7E5-79A9-5C4D-8B9F-F15347AA3655}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="3"/>
+    <col min="3" max="3" width="19.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="17.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -497,19 +511,54 @@
         <v>79122109350</v>
       </c>
       <c r="B3" s="3">
-        <v>-1490.76</v>
+        <v>-2038.91</v>
       </c>
       <c r="C3" s="3">
-        <v>-16207.56</v>
-      </c>
-      <c r="D3" s="3">
-        <v>-15992.57</v>
-      </c>
-      <c r="E3">
-        <v>-16483.77</v>
-      </c>
-      <c r="F3">
-        <v>-16168.47</v>
+        <v>-2038.92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>56100443116</v>
+      </c>
+      <c r="B4" s="3">
+        <v>4988.32</v>
+      </c>
+      <c r="C4" s="3">
+        <v>6199.34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>58101351196</v>
+      </c>
+      <c r="B5" s="3">
+        <v>559.04</v>
+      </c>
+      <c r="C5" s="3">
+        <v>-1271.1300000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>68042050362</v>
+      </c>
+      <c r="B6" s="3">
+        <v>-72081.72</v>
+      </c>
+      <c r="C6" s="3">
+        <v>-75266.48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>59093055145</v>
+      </c>
+      <c r="B7" s="3">
+        <v>3591.83</v>
+      </c>
+      <c r="C7" s="3">
+        <v>17781.13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Include updates 3 globalization Excels Bofidi
</commit_message>
<xml_diff>
--- a/excel_tax_calculation/input_output/input_output_overview.xlsx
+++ b/excel_tax_calculation/input_output/input_output_overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benjamin.van.dam/Documents/codebases/be_market/excel_tax_calculation/input_output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{806E30C0-E8B6-A147-B2E3-D77ED876C224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99E22521-ADDE-F147-8F3C-318387DBD70A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="16280" xr2:uid="{B5C74626-8E96-454A-A0EA-D4ED5FC94566}"/>
   </bookViews>
@@ -465,7 +465,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -516,6 +516,15 @@
       <c r="C3" s="3">
         <v>-2038.92</v>
       </c>
+      <c r="D3" s="3">
+        <v>-1823.9272228992447</v>
+      </c>
+      <c r="E3" s="3">
+        <v>-1721.1270833989984</v>
+      </c>
+      <c r="F3" s="3">
+        <v>-1999.8353116116334</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
@@ -525,7 +534,16 @@
         <v>4988.32</v>
       </c>
       <c r="C4" s="3">
-        <v>6199.34</v>
+        <v>5711.4209073743714</v>
+      </c>
+      <c r="D4" s="3">
+        <v>4650.488621732502</v>
+      </c>
+      <c r="E4" s="3">
+        <v>5279.5877045758834</v>
+      </c>
+      <c r="F4" s="3">
+        <v>5280.2566044854921</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -538,6 +556,15 @@
       <c r="C5" s="3">
         <v>-1271.1300000000001</v>
       </c>
+      <c r="D5" s="3">
+        <v>-23404.131545167438</v>
+      </c>
+      <c r="E5" s="3">
+        <v>-1271.1217576267572</v>
+      </c>
+      <c r="F5" s="3">
+        <v>-23404.131545167438</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
@@ -549,6 +576,15 @@
       <c r="C6" s="3">
         <v>-75266.48</v>
       </c>
+      <c r="D6" s="3">
+        <v>-75551.943901742939</v>
+      </c>
+      <c r="E6" s="3">
+        <v>-75551.943901742939</v>
+      </c>
+      <c r="F6" s="3">
+        <v>-75551.943901742939</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
@@ -559,6 +595,15 @@
       </c>
       <c r="C7" s="3">
         <v>17781.13</v>
+      </c>
+      <c r="D7" s="3">
+        <v>-20987.965400176996</v>
+      </c>
+      <c r="E7" s="3">
+        <v>22886.218720182835</v>
+      </c>
+      <c r="F7" s="3">
+        <v>-16793.762565254285</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add output pdfs and update input_output_overview
</commit_message>
<xml_diff>
--- a/excel_tax_calculation/input_output/input_output_overview.xlsx
+++ b/excel_tax_calculation/input_output/input_output_overview.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10119"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benjamin.van.dam/Documents/pit/Tax Calculation/Tests/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B250A0D-1B5C-3E43-B97B-C96F47953BC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="8">
   <si>
     <t>Input</t>
   </si>
@@ -43,8 +49,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -81,13 +87,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -125,7 +139,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -159,6 +173,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -193,9 +208,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -368,14 +384,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -401,134 +427,264 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
+        <v>68042050362</v>
+      </c>
+      <c r="B2">
+        <v>-72081.72</v>
+      </c>
+      <c r="C2">
+        <v>-72049.040000000008</v>
+      </c>
+      <c r="D2">
+        <v>-72049.040000000008</v>
+      </c>
+      <c r="E2">
+        <v>-72046.83</v>
+      </c>
+      <c r="F2">
+        <v>-72049.040000000008</v>
+      </c>
+      <c r="G2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2">
+        <v>32.679999999993015</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>80080764310</v>
+      </c>
+      <c r="B3">
+        <v>82.01</v>
+      </c>
+      <c r="C3">
+        <v>110.21</v>
+      </c>
+      <c r="D3">
+        <v>90.58</v>
+      </c>
+      <c r="E3">
+        <v>90.58</v>
+      </c>
+      <c r="F3">
+        <v>90.58</v>
+      </c>
+      <c r="G3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3">
+        <v>8.5699999999999932</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>80091134994</v>
+      </c>
+      <c r="B4">
+        <v>957.75</v>
+      </c>
+      <c r="C4">
+        <v>-2050.44</v>
+      </c>
+      <c r="D4">
+        <v>-2050.44</v>
+      </c>
+      <c r="E4">
+        <v>-1732.65</v>
+      </c>
+      <c r="F4">
+        <v>-2050.44</v>
+      </c>
+      <c r="G4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4">
+        <v>2690.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>79122109350</v>
+      </c>
+      <c r="B5">
+        <v>-2038.91</v>
+      </c>
+      <c r="C5">
+        <v>-2042.75</v>
+      </c>
+      <c r="D5">
+        <v>-2003.41</v>
+      </c>
+      <c r="E5">
+        <v>-1724.96</v>
+      </c>
+      <c r="F5">
+        <v>-2003.41</v>
+      </c>
+      <c r="G5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <v>3.8399999999999181</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>58101351196</v>
+      </c>
+      <c r="B6">
+        <v>559.04</v>
+      </c>
+      <c r="C6">
+        <v>1072.96</v>
+      </c>
+      <c r="D6">
+        <v>-28294.34</v>
+      </c>
+      <c r="E6">
+        <v>1074.3500000000004</v>
+      </c>
+      <c r="F6">
+        <v>-28294.34</v>
+      </c>
+      <c r="G6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6">
+        <v>513.92000000000007</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>70062422978</v>
+      </c>
+      <c r="B7">
+        <v>5457.95</v>
+      </c>
+      <c r="C7">
+        <v>-4368.26</v>
+      </c>
+      <c r="D7">
+        <v>-7895.41</v>
+      </c>
+      <c r="E7">
+        <v>-7895.41</v>
+      </c>
+      <c r="F7">
+        <v>-7895.41</v>
+      </c>
+      <c r="G7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7">
+        <v>9826.2099999999991</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>89051637777</v>
+      </c>
+      <c r="B8">
+        <v>3627.39</v>
+      </c>
+      <c r="C8">
+        <v>-2537.71</v>
+      </c>
+      <c r="D8">
+        <v>-6064.86</v>
+      </c>
+      <c r="E8">
+        <v>-5747.07</v>
+      </c>
+      <c r="F8">
+        <v>-6064.86</v>
+      </c>
+      <c r="G8" t="s">
+        <v>2</v>
+      </c>
+      <c r="H8">
+        <v>6165.1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9">
         <v>56100443116</v>
       </c>
-      <c r="B2">
+      <c r="B9">
         <v>4988.32</v>
       </c>
-      <c r="C2">
+      <c r="C9">
         <v>4988.3099999999995</v>
       </c>
-      <c r="D2">
+      <c r="D9">
         <v>4988.83</v>
       </c>
-      <c r="E2">
+      <c r="E9">
         <v>4988.2300000000005</v>
       </c>
-      <c r="F2">
-        <v>4988.889999999999</v>
-      </c>
-      <c r="G2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H2">
-        <v>0.010000000000218279</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3">
-        <v>79122109350</v>
-      </c>
-      <c r="B3">
-        <v>-2038.91</v>
-      </c>
-      <c r="C3">
-        <v>-2042.75</v>
-      </c>
-      <c r="D3">
-        <v>-2003.41</v>
-      </c>
-      <c r="E3">
-        <v>-1724.96</v>
-      </c>
-      <c r="F3">
-        <v>-2003.41</v>
-      </c>
-      <c r="G3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3">
-        <v>3.839999999999918</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4">
-        <v>58101351196</v>
-      </c>
-      <c r="B4">
-        <v>559.04</v>
-      </c>
-      <c r="C4">
-        <v>1072.96</v>
-      </c>
-      <c r="D4">
-        <v>-28294.34</v>
-      </c>
-      <c r="E4">
-        <v>1074.3500000000004</v>
-      </c>
-      <c r="F4">
-        <v>-28294.34</v>
-      </c>
-      <c r="G4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H4">
-        <v>513.9200000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5">
+      <c r="F9">
+        <v>4988.8899999999994</v>
+      </c>
+      <c r="G9" t="s">
+        <v>2</v>
+      </c>
+      <c r="H9">
+        <v>1.0000000000218279E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>91042947017</v>
+      </c>
+      <c r="B10">
+        <v>71698.31</v>
+      </c>
+      <c r="C10">
+        <v>71454.58</v>
+      </c>
+      <c r="D10">
+        <v>67630.53</v>
+      </c>
+      <c r="E10">
+        <v>67961.070000000007</v>
+      </c>
+      <c r="F10">
+        <v>67630.53</v>
+      </c>
+      <c r="G10" t="s">
+        <v>2</v>
+      </c>
+      <c r="H10">
+        <v>243.72999999999593</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11">
         <v>59093055145</v>
       </c>
-      <c r="B5">
+      <c r="B11">
         <v>3591.83</v>
       </c>
-      <c r="C5">
+      <c r="C11">
         <v>1535.6500000000005</v>
       </c>
-      <c r="D5">
-        <v>-41497.71000000001</v>
-      </c>
-      <c r="E5">
+      <c r="D11">
+        <v>-41497.710000000006</v>
+      </c>
+      <c r="E11">
         <v>2411.2799999999997</v>
       </c>
-      <c r="F5">
+      <c r="F11">
         <v>-52406.91</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G11" t="s">
         <v>4</v>
       </c>
-      <c r="H5">
+      <c r="H11">
         <v>1180.5500000000002</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6">
-        <v>68042050362</v>
-      </c>
-      <c r="B6">
-        <v>-72081.72</v>
-      </c>
-      <c r="C6">
-        <v>-72049.04000000001</v>
-      </c>
-      <c r="D6">
-        <v>-72049.04000000001</v>
-      </c>
-      <c r="E6">
-        <v>-72046.83</v>
-      </c>
-      <c r="F6">
-        <v>-72049.04000000001</v>
-      </c>
-      <c r="G6" t="s">
-        <v>2</v>
-      </c>
-      <c r="H6">
-        <v>32.679999999993015</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corrected jsons to use SF version instead of TPI version
</commit_message>
<xml_diff>
--- a/excel_tax_calculation/input_output/input_output_overview.xlsx
+++ b/excel_tax_calculation/input_output/input_output_overview.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10119"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benjamin.van.dam/Documents/pit/Tax Calculation/Tests/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B250A0D-1B5C-3E43-B97B-C96F47953BC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -49,8 +43,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -87,21 +81,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -139,7 +125,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -173,7 +159,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -208,10 +193,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -384,24 +368,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.33203125" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -427,33 +401,33 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8">
       <c r="A2">
-        <v>68042050362</v>
+        <v>56100443116</v>
       </c>
       <c r="B2">
-        <v>-72081.72</v>
+        <v>4988.32</v>
       </c>
       <c r="C2">
-        <v>-72049.040000000008</v>
+        <v>4988.3099999999995</v>
       </c>
       <c r="D2">
-        <v>-72049.040000000008</v>
+        <v>4988.83</v>
       </c>
       <c r="E2">
-        <v>-72046.83</v>
+        <v>4988.2300000000005</v>
       </c>
       <c r="F2">
-        <v>-72049.040000000008</v>
+        <v>4988.889999999999</v>
       </c>
       <c r="G2" t="s">
         <v>2</v>
       </c>
       <c r="H2">
-        <v>32.679999999993015</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+        <v>0.010000000000218279</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3">
         <v>80080764310</v>
       </c>
@@ -476,62 +450,62 @@
         <v>3</v>
       </c>
       <c r="H3">
-        <v>8.5699999999999932</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+        <v>8.569999999999993</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4">
-        <v>80091134994</v>
+        <v>70062422978</v>
       </c>
       <c r="B4">
-        <v>957.75</v>
+        <v>5457.95</v>
       </c>
       <c r="C4">
-        <v>-2050.44</v>
+        <v>-6106.37</v>
       </c>
       <c r="D4">
-        <v>-2050.44</v>
+        <v>-6106.37</v>
       </c>
       <c r="E4">
-        <v>-1732.65</v>
+        <v>-6106.37</v>
       </c>
       <c r="F4">
-        <v>-2050.44</v>
+        <v>-6106.37</v>
       </c>
       <c r="G4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H4">
-        <v>2690.4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+        <v>11564.32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5">
-        <v>79122109350</v>
+        <v>91042947017</v>
       </c>
       <c r="B5">
-        <v>-2038.91</v>
+        <v>71698.31</v>
       </c>
       <c r="C5">
-        <v>-2042.75</v>
+        <v>71698.32</v>
       </c>
       <c r="D5">
-        <v>-2003.41</v>
+        <v>71698.32</v>
       </c>
       <c r="E5">
-        <v>-1724.96</v>
+        <v>72028.86</v>
       </c>
       <c r="F5">
-        <v>-2003.41</v>
+        <v>71698.32</v>
       </c>
       <c r="G5" t="s">
         <v>2</v>
       </c>
       <c r="H5">
-        <v>3.8399999999999181</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+        <v>0.010000000009313226</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6">
         <v>58101351196</v>
       </c>
@@ -554,137 +528,137 @@
         <v>2</v>
       </c>
       <c r="H6">
-        <v>513.92000000000007</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+        <v>513.9200000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7">
-        <v>70062422978</v>
+        <v>89051637777</v>
       </c>
       <c r="B7">
-        <v>5457.95</v>
+        <v>3627.39</v>
       </c>
       <c r="C7">
-        <v>-4368.26</v>
+        <v>-4275.82</v>
       </c>
       <c r="D7">
-        <v>-7895.41</v>
+        <v>-4275.82</v>
       </c>
       <c r="E7">
-        <v>-7895.41</v>
+        <v>-3958.03</v>
       </c>
       <c r="F7">
-        <v>-7895.41</v>
+        <v>-4275.82</v>
       </c>
       <c r="G7" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H7">
-        <v>9826.2099999999991</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+        <v>7585.42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8">
-        <v>89051637777</v>
+        <v>68042050362</v>
       </c>
       <c r="B8">
-        <v>3627.39</v>
+        <v>-72081.72</v>
       </c>
       <c r="C8">
-        <v>-2537.71</v>
+        <v>-72049.04000000001</v>
       </c>
       <c r="D8">
-        <v>-6064.86</v>
+        <v>-72049.04000000001</v>
       </c>
       <c r="E8">
-        <v>-5747.07</v>
+        <v>-72046.83</v>
       </c>
       <c r="F8">
-        <v>-6064.86</v>
+        <v>-72049.04000000001</v>
       </c>
       <c r="G8" t="s">
         <v>2</v>
       </c>
       <c r="H8">
-        <v>6165.1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+        <v>32.679999999993015</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9">
-        <v>56100443116</v>
+        <v>59093055145</v>
       </c>
       <c r="B9">
-        <v>4988.32</v>
+        <v>3591.83</v>
       </c>
       <c r="C9">
-        <v>4988.3099999999995</v>
+        <v>1535.6500000000005</v>
       </c>
       <c r="D9">
-        <v>4988.83</v>
+        <v>-41497.71000000001</v>
       </c>
       <c r="E9">
-        <v>4988.2300000000005</v>
+        <v>2411.2799999999997</v>
       </c>
       <c r="F9">
-        <v>4988.8899999999994</v>
+        <v>-52406.91</v>
       </c>
       <c r="G9" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H9">
-        <v>1.0000000000218279E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+        <v>1180.5500000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10">
-        <v>91042947017</v>
+        <v>79122109350</v>
       </c>
       <c r="B10">
-        <v>71698.31</v>
+        <v>-2038.91</v>
       </c>
       <c r="C10">
-        <v>71454.58</v>
+        <v>-2042.75</v>
       </c>
       <c r="D10">
-        <v>67630.53</v>
+        <v>-2003.41</v>
       </c>
       <c r="E10">
-        <v>67961.070000000007</v>
+        <v>-1724.96</v>
       </c>
       <c r="F10">
-        <v>67630.53</v>
+        <v>-2003.41</v>
       </c>
       <c r="G10" t="s">
         <v>2</v>
       </c>
       <c r="H10">
-        <v>243.72999999999593</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+        <v>3.839999999999918</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11">
-        <v>59093055145</v>
+        <v>80091134994</v>
       </c>
       <c r="B11">
-        <v>3591.83</v>
+        <v>957.75</v>
       </c>
       <c r="C11">
-        <v>1535.6500000000005</v>
+        <v>-2050.44</v>
       </c>
       <c r="D11">
-        <v>-41497.710000000006</v>
+        <v>-2050.44</v>
       </c>
       <c r="E11">
-        <v>2411.2799999999997</v>
+        <v>-1732.65</v>
       </c>
       <c r="F11">
-        <v>-52406.91</v>
+        <v>-2050.44</v>
       </c>
       <c r="G11" t="s">
         <v>4</v>
       </c>
       <c r="H11">
-        <v>1180.5500000000002</v>
+        <v>2690.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Include additional calculations for Bofidi
</commit_message>
<xml_diff>
--- a/excel_tax_calculation/input_output/input_output_overview.xlsx
+++ b/excel_tax_calculation/input_output/input_output_overview.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10119"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benjamin.van.dam/Documents/codebases/be_market/excel_tax_calculation/input_output/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71E87D9D-6DBB-524A-9FA1-58E37893BB00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="28800" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="8">
   <si>
     <t>Input</t>
   </si>
@@ -43,8 +49,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -53,12 +59,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -73,21 +91,31 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -125,7 +153,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -159,6 +187,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -193,9 +222,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -368,14 +398,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -401,264 +441,394 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
+        <v>68042050362</v>
+      </c>
+      <c r="B2">
+        <v>-72081.72</v>
+      </c>
+      <c r="C2">
+        <v>-72049.040000000008</v>
+      </c>
+      <c r="D2">
+        <v>-72049.040000000008</v>
+      </c>
+      <c r="E2">
+        <v>-77999.3</v>
+      </c>
+      <c r="F2">
+        <v>-72049.040000000008</v>
+      </c>
+      <c r="G2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2">
+        <v>32.679999999993015</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>70062422978</v>
+      </c>
+      <c r="B3">
+        <v>-5457.95</v>
+      </c>
+      <c r="C3">
+        <v>-5457.95</v>
+      </c>
+      <c r="D3">
+        <v>-5457.95</v>
+      </c>
+      <c r="E3">
+        <v>-26431.61</v>
+      </c>
+      <c r="F3">
+        <v>-5457.95</v>
+      </c>
+      <c r="G3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>65122716289</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
+        <v>-820</v>
+      </c>
+      <c r="D4" s="1">
+        <v>-820</v>
+      </c>
+      <c r="E4" s="1">
+        <v>-6182.83</v>
+      </c>
+      <c r="F4" s="1">
+        <v>-820</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="1">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>59093055145</v>
+      </c>
+      <c r="B5">
+        <v>3591.83</v>
+      </c>
+      <c r="C5">
+        <v>1535.6500000000005</v>
+      </c>
+      <c r="D5">
+        <v>-41497.710000000006</v>
+      </c>
+      <c r="E5">
+        <v>3866.08</v>
+      </c>
+      <c r="F5">
+        <v>-52406.91</v>
+      </c>
+      <c r="G5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5">
+        <v>274.25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6">
         <v>56100443116</v>
       </c>
-      <c r="B2">
+      <c r="B6">
         <v>4988.32</v>
       </c>
-      <c r="C2">
+      <c r="C6">
         <v>4988.3099999999995</v>
       </c>
-      <c r="D2">
+      <c r="D6">
         <v>4988.83</v>
       </c>
-      <c r="E2">
-        <v>4988.2300000000005</v>
-      </c>
-      <c r="F2">
-        <v>4988.889999999999</v>
-      </c>
-      <c r="G2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H2">
-        <v>0.010000000000218279</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3">
+      <c r="E6">
+        <v>9673.4700000000012</v>
+      </c>
+      <c r="F6">
+        <v>4988.8899999999994</v>
+      </c>
+      <c r="G6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6">
+        <v>1.0000000000218279E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7">
         <v>80080764310</v>
       </c>
-      <c r="B3">
+      <c r="B7">
         <v>82.01</v>
       </c>
-      <c r="C3">
-        <v>110.21</v>
-      </c>
-      <c r="D3">
-        <v>90.58</v>
-      </c>
-      <c r="E3">
-        <v>90.58</v>
-      </c>
-      <c r="F3">
-        <v>90.58</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="C7">
+        <v>82.01</v>
+      </c>
+      <c r="D7">
+        <v>82.01</v>
+      </c>
+      <c r="E7">
+        <v>-7788.55</v>
+      </c>
+      <c r="F7">
+        <v>82.01</v>
+      </c>
+      <c r="G7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>91042947017</v>
+      </c>
+      <c r="B8">
+        <v>71698.31</v>
+      </c>
+      <c r="C8">
+        <v>71698.320000000007</v>
+      </c>
+      <c r="D8">
+        <v>71698.320000000007</v>
+      </c>
+      <c r="E8">
+        <v>34887.74</v>
+      </c>
+      <c r="F8">
+        <v>71698.320000000007</v>
+      </c>
+      <c r="G8" t="s">
+        <v>2</v>
+      </c>
+      <c r="H8">
+        <v>1.0000000009313226E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>79122109350</v>
+      </c>
+      <c r="B9">
+        <v>-2038.91</v>
+      </c>
+      <c r="C9">
+        <v>-2042.75</v>
+      </c>
+      <c r="D9">
+        <v>-2003.41</v>
+      </c>
+      <c r="E9">
+        <v>-23363.599999999999</v>
+      </c>
+      <c r="F9">
+        <v>-2003.41</v>
+      </c>
+      <c r="G9" t="s">
+        <v>2</v>
+      </c>
+      <c r="H9">
+        <v>3.8399999999999181</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>65052932511</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1176.55</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1027</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1027</v>
+      </c>
+      <c r="E10" s="1">
+        <v>-36354.870000000003</v>
+      </c>
+      <c r="F10" s="1">
+        <v>1079.96</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H10" s="1">
+        <v>96.589999999999918</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>73061516983</v>
+      </c>
+      <c r="B11" s="1">
+        <v>-2011.08</v>
+      </c>
+      <c r="C11" s="1">
+        <v>-2031.92</v>
+      </c>
+      <c r="D11" s="1">
+        <v>-1974.7400000000002</v>
+      </c>
+      <c r="E11" s="1">
+        <v>-28573.019999999997</v>
+      </c>
+      <c r="F11" s="1">
+        <v>-1867.08</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H11" s="1">
+        <v>20.840000000000146</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>86080827685</v>
+      </c>
+      <c r="B12" s="1">
+        <v>-3098.48</v>
+      </c>
+      <c r="C12" s="1">
+        <v>-3442.34</v>
+      </c>
+      <c r="D12" s="1">
+        <v>-3127.38</v>
+      </c>
+      <c r="E12" s="1">
+        <v>-38729.620000000003</v>
+      </c>
+      <c r="F12" s="1">
+        <v>-2831.69</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H3">
-        <v>8.569999999999993</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4">
-        <v>70062422978</v>
-      </c>
-      <c r="B4">
-        <v>5457.95</v>
-      </c>
-      <c r="C4">
-        <v>-6106.37</v>
-      </c>
-      <c r="D4">
-        <v>-6106.37</v>
-      </c>
-      <c r="E4">
-        <v>-6106.37</v>
-      </c>
-      <c r="F4">
-        <v>-6106.37</v>
-      </c>
-      <c r="G4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H4">
-        <v>11564.32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5">
-        <v>91042947017</v>
-      </c>
-      <c r="B5">
-        <v>71698.31</v>
-      </c>
-      <c r="C5">
-        <v>71698.32</v>
-      </c>
-      <c r="D5">
-        <v>71698.32</v>
-      </c>
-      <c r="E5">
-        <v>72028.86</v>
-      </c>
-      <c r="F5">
-        <v>71698.32</v>
-      </c>
-      <c r="G5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H5">
-        <v>0.010000000009313226</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6">
+      <c r="H12" s="1">
+        <v>28.900000000000091</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
+        <v>80120831347</v>
+      </c>
+      <c r="B13" s="2">
+        <v>-2701.23</v>
+      </c>
+      <c r="C13" s="2">
+        <v>-2701.22</v>
+      </c>
+      <c r="D13" s="2">
+        <v>-2701.22</v>
+      </c>
+      <c r="E13" s="2">
+        <v>-35769.740000000005</v>
+      </c>
+      <c r="F13" s="2">
+        <v>-2696.7999999999997</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H13" s="2">
+        <v>1.0000000000218279E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14">
         <v>58101351196</v>
       </c>
-      <c r="B6">
+      <c r="B14">
         <v>559.04</v>
       </c>
-      <c r="C6">
-        <v>1072.96</v>
-      </c>
-      <c r="D6">
-        <v>-28294.34</v>
-      </c>
-      <c r="E6">
-        <v>1074.3500000000004</v>
-      </c>
-      <c r="F6">
-        <v>-28294.34</v>
-      </c>
-      <c r="G6" t="s">
-        <v>2</v>
-      </c>
-      <c r="H6">
-        <v>513.9200000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7">
+      <c r="C14">
+        <v>1077.9400000000005</v>
+      </c>
+      <c r="D14">
+        <v>-28289.289999999997</v>
+      </c>
+      <c r="E14">
+        <v>-7640.5</v>
+      </c>
+      <c r="F14">
+        <v>-28289.289999999997</v>
+      </c>
+      <c r="G14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H14">
+        <v>518.90000000000055</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15">
         <v>89051637777</v>
       </c>
-      <c r="B7">
-        <v>3627.39</v>
-      </c>
-      <c r="C7">
-        <v>-4275.82</v>
-      </c>
-      <c r="D7">
-        <v>-4275.82</v>
-      </c>
-      <c r="E7">
-        <v>-3958.03</v>
-      </c>
-      <c r="F7">
-        <v>-4275.82</v>
-      </c>
-      <c r="G7" t="s">
-        <v>4</v>
-      </c>
-      <c r="H7">
-        <v>7585.42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8">
-        <v>68042050362</v>
-      </c>
-      <c r="B8">
-        <v>-72081.72</v>
-      </c>
-      <c r="C8">
-        <v>-72049.04000000001</v>
-      </c>
-      <c r="D8">
-        <v>-72049.04000000001</v>
-      </c>
-      <c r="E8">
-        <v>-72046.83</v>
-      </c>
-      <c r="F8">
-        <v>-72049.04000000001</v>
-      </c>
-      <c r="G8" t="s">
-        <v>2</v>
-      </c>
-      <c r="H8">
-        <v>32.679999999993015</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9">
-        <v>59093055145</v>
-      </c>
-      <c r="B9">
-        <v>3591.83</v>
-      </c>
-      <c r="C9">
-        <v>1535.6500000000005</v>
-      </c>
-      <c r="D9">
-        <v>-41497.71000000001</v>
-      </c>
-      <c r="E9">
-        <v>2411.2799999999997</v>
-      </c>
-      <c r="F9">
-        <v>-52406.91</v>
-      </c>
-      <c r="G9" t="s">
-        <v>4</v>
-      </c>
-      <c r="H9">
-        <v>1180.5500000000002</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10">
-        <v>79122109350</v>
-      </c>
-      <c r="B10">
-        <v>-2038.91</v>
-      </c>
-      <c r="C10">
-        <v>-2042.75</v>
-      </c>
-      <c r="D10">
-        <v>-2003.41</v>
-      </c>
-      <c r="E10">
-        <v>-1724.96</v>
-      </c>
-      <c r="F10">
-        <v>-2003.41</v>
-      </c>
-      <c r="G10" t="s">
-        <v>2</v>
-      </c>
-      <c r="H10">
-        <v>3.839999999999918</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11">
+      <c r="B15">
+        <v>-3627.39</v>
+      </c>
+      <c r="C15">
+        <v>-3627.4</v>
+      </c>
+      <c r="D15">
+        <v>-3627.4</v>
+      </c>
+      <c r="E15">
+        <v>-26584.18</v>
+      </c>
+      <c r="F15">
+        <v>-3627.4</v>
+      </c>
+      <c r="G15" t="s">
+        <v>2</v>
+      </c>
+      <c r="H15">
+        <v>1.0000000000218279E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16">
         <v>80091134994</v>
       </c>
-      <c r="B11">
-        <v>957.75</v>
-      </c>
-      <c r="C11">
+      <c r="B16">
+        <v>-2050.4299999999998</v>
+      </c>
+      <c r="C16">
         <v>-2050.44</v>
       </c>
-      <c r="D11">
+      <c r="D16">
         <v>-2050.44</v>
       </c>
-      <c r="E11">
-        <v>-1732.65</v>
-      </c>
-      <c r="F11">
+      <c r="E16">
+        <v>-34574.69</v>
+      </c>
+      <c r="F16">
         <v>-2050.44</v>
       </c>
-      <c r="G11" t="s">
-        <v>4</v>
-      </c>
-      <c r="H11">
-        <v>2690.4</v>
+      <c r="G16" t="s">
+        <v>2</v>
+      </c>
+      <c r="H16">
+        <v>1.0000000000218279E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>